<commit_message>
Create  one EM file, almost handling missing values correctly
</commit_message>
<xml_diff>
--- a/Block_WBC.xlsx
+++ b/Block_WBC.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\sambaad.stud.ntnu.no\sigvekb\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sigvekb\Master\dynamic-factor\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="B1" sheetId="1" r:id="rId1"/>
+    <sheet name="B2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
   <si>
     <t>Platinum</t>
   </si>
@@ -551,8 +552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,7 +601,7 @@
         <v>56</v>
       </c>
       <c r="K1">
-        <f>COUNTIF($A$2:$I$18,L1)</f>
+        <f t="shared" ref="K1:K32" si="0">COUNTIF($A$2:$I$18,L1)</f>
         <v>1</v>
       </c>
       <c r="L1" s="1">
@@ -639,7 +640,7 @@
         <v>54</v>
       </c>
       <c r="K2">
-        <f>COUNTIF($A$2:$I$18,L2)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L2" s="1">
@@ -678,7 +679,7 @@
         <v>55</v>
       </c>
       <c r="K3">
-        <f>COUNTIF($A$2:$I$18,L3)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L3" s="1">
@@ -717,7 +718,7 @@
         <v>56</v>
       </c>
       <c r="K4">
-        <f>COUNTIF($A$2:$I$18,L4)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L4" s="1">
@@ -754,7 +755,7 @@
       </c>
       <c r="I5" s="2"/>
       <c r="K5">
-        <f>COUNTIF($A$2:$I$18,L5)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L5" s="1">
@@ -789,7 +790,7 @@
       </c>
       <c r="I6" s="2"/>
       <c r="K6">
-        <f>COUNTIF($A$2:$I$18,L6)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L6" s="1">
@@ -822,7 +823,7 @@
       </c>
       <c r="I7" s="2"/>
       <c r="K7">
-        <f>COUNTIF($A$2:$I$18,L7)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L7" s="1">
@@ -853,7 +854,7 @@
       </c>
       <c r="I8" s="2"/>
       <c r="K8">
-        <f>COUNTIF($A$2:$I$18,L8)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L8" s="1">
@@ -878,7 +879,7 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="K9">
-        <f>COUNTIF($A$2:$I$18,L9)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L9" s="1">
@@ -901,7 +902,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="K10">
-        <f>COUNTIF($A$2:$I$18,L10)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L10" s="1">
@@ -922,7 +923,7 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="K11">
-        <f>COUNTIF($A$2:$I$18,L11)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L11" s="1">
@@ -943,7 +944,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="K12">
-        <f>COUNTIF($A$2:$I$18,L12)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L12" s="1">
@@ -964,7 +965,7 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="K13">
-        <f>COUNTIF($A$2:$I$18,L13)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L13" s="1">
@@ -985,7 +986,7 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="K14">
-        <f>COUNTIF($A$2:$I$18,L14)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L14" s="1">
@@ -1006,7 +1007,7 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="K15">
-        <f>COUNTIF($A$2:$I$18,L15)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L15" s="1">
@@ -1027,7 +1028,7 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="K16">
-        <f>COUNTIF($A$2:$I$18,L16)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L16" s="1">
@@ -1048,7 +1049,7 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="K17">
-        <f>COUNTIF($A$2:$I$18,L17)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L17" s="1">
@@ -1069,7 +1070,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="K18">
-        <f>COUNTIF($A$2:$I$18,L18)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L18" s="1">
@@ -1090,7 +1091,7 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="K19">
-        <f>COUNTIF($A$2:$I$18,L19)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L19" s="1">
@@ -1111,7 +1112,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="K20">
-        <f>COUNTIF($A$2:$I$18,L20)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L20" s="1">
@@ -1132,7 +1133,7 @@
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="K21">
-        <f>COUNTIF($A$2:$I$18,L21)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L21" s="1">
@@ -1153,7 +1154,7 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="K22">
-        <f>COUNTIF($A$2:$I$18,L22)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L22" s="1">
@@ -1165,7 +1166,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K23">
-        <f>COUNTIF($A$2:$I$18,L23)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L23" s="1">
@@ -1177,7 +1178,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K24">
-        <f>COUNTIF($A$2:$I$18,L24)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L24" s="1">
@@ -1189,7 +1190,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K25">
-        <f>COUNTIF($A$2:$I$18,L25)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L25" s="1">
@@ -1201,7 +1202,7 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K26">
-        <f>COUNTIF($A$2:$I$18,L26)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L26" s="1">
@@ -1213,7 +1214,7 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K27">
-        <f>COUNTIF($A$2:$I$18,L27)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L27" s="1">
@@ -1225,7 +1226,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K28">
-        <f>COUNTIF($A$2:$I$18,L28)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L28" s="1">
@@ -1237,7 +1238,7 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K29">
-        <f>COUNTIF($A$2:$I$18,L29)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L29" s="1">
@@ -1249,7 +1250,7 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K30">
-        <f>COUNTIF($A$2:$I$18,L30)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L30" s="1">
@@ -1261,7 +1262,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K31">
-        <f>COUNTIF($A$2:$I$18,L31)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L31" s="1">
@@ -1273,7 +1274,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K32">
-        <f>COUNTIF($A$2:$I$18,L32)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L32" s="1">
@@ -1285,7 +1286,7 @@
     </row>
     <row r="33" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K33">
-        <f>COUNTIF($A$2:$I$18,L33)</f>
+        <f t="shared" ref="K33:K64" si="1">COUNTIF($A$2:$I$18,L33)</f>
         <v>1</v>
       </c>
       <c r="L33" s="1">
@@ -1297,7 +1298,7 @@
     </row>
     <row r="34" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K34">
-        <f>COUNTIF($A$2:$I$18,L34)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L34" s="1">
@@ -1309,7 +1310,7 @@
     </row>
     <row r="35" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K35">
-        <f>COUNTIF($A$2:$I$18,L35)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L35" s="1">
@@ -1321,7 +1322,7 @@
     </row>
     <row r="36" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K36">
-        <f>COUNTIF($A$2:$I$18,L36)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L36" s="1">
@@ -1333,7 +1334,7 @@
     </row>
     <row r="37" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K37">
-        <f>COUNTIF($A$2:$I$18,L37)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L37" s="1">
@@ -1345,7 +1346,7 @@
     </row>
     <row r="38" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K38">
-        <f>COUNTIF($A$2:$I$18,L38)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L38" s="1">
@@ -1357,7 +1358,7 @@
     </row>
     <row r="39" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K39">
-        <f>COUNTIF($A$2:$I$18,L39)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L39" s="1">
@@ -1369,7 +1370,7 @@
     </row>
     <row r="40" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K40">
-        <f>COUNTIF($A$2:$I$18,L40)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L40" s="1">
@@ -1381,7 +1382,7 @@
     </row>
     <row r="41" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K41">
-        <f>COUNTIF($A$2:$I$18,L41)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L41" s="1">
@@ -1393,7 +1394,7 @@
     </row>
     <row r="42" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K42">
-        <f>COUNTIF($A$2:$I$18,L42)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L42" s="1">
@@ -1405,7 +1406,7 @@
     </row>
     <row r="43" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K43">
-        <f>COUNTIF($A$2:$I$18,L43)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L43" s="1">
@@ -1417,7 +1418,7 @@
     </row>
     <row r="44" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K44">
-        <f>COUNTIF($A$2:$I$18,L44)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L44" s="1">
@@ -1429,7 +1430,7 @@
     </row>
     <row r="45" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K45">
-        <f>COUNTIF($A$2:$I$18,L45)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L45" s="1">
@@ -1441,7 +1442,7 @@
     </row>
     <row r="46" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K46">
-        <f>COUNTIF($A$2:$I$18,L46)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L46" s="1">
@@ -1453,7 +1454,7 @@
     </row>
     <row r="47" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K47">
-        <f>COUNTIF($A$2:$I$18,L47)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L47" s="1">
@@ -1465,7 +1466,7 @@
     </row>
     <row r="48" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K48">
-        <f>COUNTIF($A$2:$I$18,L48)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L48" s="1">
@@ -1477,7 +1478,7 @@
     </row>
     <row r="49" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K49">
-        <f>COUNTIF($A$2:$I$18,L49)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L49" s="1">
@@ -1489,7 +1490,7 @@
     </row>
     <row r="50" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K50">
-        <f>COUNTIF($A$2:$I$18,L50)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L50" s="1">
@@ -1501,7 +1502,7 @@
     </row>
     <row r="51" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K51">
-        <f>COUNTIF($A$2:$I$18,L51)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L51" s="1">
@@ -1513,7 +1514,7 @@
     </row>
     <row r="52" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K52">
-        <f>COUNTIF($A$2:$I$18,L52)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L52" s="1">
@@ -1525,7 +1526,7 @@
     </row>
     <row r="53" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K53">
-        <f>COUNTIF($A$2:$I$18,L53)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L53" s="1">
@@ -1537,7 +1538,7 @@
     </row>
     <row r="54" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K54">
-        <f>COUNTIF($A$2:$I$18,L54)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L54" s="1">
@@ -1549,7 +1550,7 @@
     </row>
     <row r="55" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K55">
-        <f>COUNTIF($A$2:$I$18,L55)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L55" s="1">
@@ -1561,7 +1562,7 @@
     </row>
     <row r="56" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K56">
-        <f>COUNTIF($A$2:$I$18,L56)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="L56" s="1">
@@ -1573,7 +1574,7 @@
     </row>
     <row r="57" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K57">
-        <f>COUNTIF($A$2:$I$18,L57)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L57" s="1">
@@ -1582,7 +1583,7 @@
     </row>
     <row r="58" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K58">
-        <f>COUNTIF($A$2:$I$18,L58)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L58" s="1">
@@ -1591,7 +1592,7 @@
     </row>
     <row r="59" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K59">
-        <f>COUNTIF($A$2:$I$18,L59)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L59" s="1">
@@ -1600,7 +1601,7 @@
     </row>
     <row r="60" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K60">
-        <f>COUNTIF($A$2:$I$18,L60)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L60" s="1">
@@ -1622,4 +1623,47 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Try removing series with ,more than 20 percent missing observations
</commit_message>
<xml_diff>
--- a/Block_WBC.xlsx
+++ b/Block_WBC.xlsx
@@ -2,20 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sigvekb\Master\dynamic-factor\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100"/>
   </bookViews>
   <sheets>
     <sheet name="B1" sheetId="1" r:id="rId1"/>
     <sheet name="B2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,18 +39,12 @@
     <t>Nickel</t>
   </si>
   <si>
-    <t>Aluminium</t>
-  </si>
-  <si>
     <t>Copper</t>
   </si>
   <si>
     <t>Lead</t>
   </si>
   <si>
-    <t xml:space="preserve">Tin </t>
-  </si>
-  <si>
     <t>Zinc</t>
   </si>
   <si>
@@ -63,9 +57,6 @@
     <t>Potassium chloride</t>
   </si>
   <si>
-    <t>Urea</t>
-  </si>
-  <si>
     <t>TSP</t>
   </si>
   <si>
@@ -96,30 +87,15 @@
     <t>PSALM</t>
   </si>
   <si>
-    <t>Surgar, World</t>
-  </si>
-  <si>
     <t>Shrimps, Mexican</t>
   </si>
   <si>
     <t>Meat, sheep</t>
   </si>
   <si>
-    <t>Meat, Chicken</t>
-  </si>
-  <si>
-    <t>beef</t>
-  </si>
-  <si>
-    <t>Fishmeal</t>
-  </si>
-  <si>
     <t>Banana, US</t>
   </si>
   <si>
-    <t>Wheat, US</t>
-  </si>
-  <si>
     <t>Sorghum</t>
   </si>
   <si>
@@ -141,18 +117,12 @@
     <t>Rapeseed oil</t>
   </si>
   <si>
-    <t xml:space="preserve">Soybean  </t>
-  </si>
-  <si>
     <t>Soybean meal</t>
   </si>
   <si>
     <t>Palm oil</t>
   </si>
   <si>
-    <t>Groundnuts oil</t>
-  </si>
-  <si>
     <t>Groundnuts</t>
   </si>
   <si>
@@ -162,39 +132,6 @@
     <t>Coconut oil</t>
   </si>
   <si>
-    <t>Tea, A.1</t>
-  </si>
-  <si>
-    <t>Coffe, Arabica</t>
-  </si>
-  <si>
-    <t>Coffe, Robusta</t>
-  </si>
-  <si>
-    <t>Cocca</t>
-  </si>
-  <si>
-    <t>LNG</t>
-  </si>
-  <si>
-    <t>Natural Gas, US</t>
-  </si>
-  <si>
-    <t>Natural Gas, EU</t>
-  </si>
-  <si>
-    <t>Crude oil Dubai</t>
-  </si>
-  <si>
-    <t>Crude oil WTI</t>
-  </si>
-  <si>
-    <t>Crude oil brent</t>
-  </si>
-  <si>
-    <t>Coal (Australia)</t>
-  </si>
-  <si>
     <t>Precious metals</t>
   </si>
   <si>
@@ -220,12 +157,75 @@
   </si>
   <si>
     <t>Energy</t>
+  </si>
+  <si>
+    <t>Crude oil, Brent</t>
+  </si>
+  <si>
+    <t>Crude oil, Dubai</t>
+  </si>
+  <si>
+    <t>Crude oil, WTI</t>
+  </si>
+  <si>
+    <t>Coal, Australian</t>
+  </si>
+  <si>
+    <t>Natural gas, US</t>
+  </si>
+  <si>
+    <t>Natural gas, Europe</t>
+  </si>
+  <si>
+    <t>Liquefied natural gas, Japan</t>
+  </si>
+  <si>
+    <t>Cocoa</t>
+  </si>
+  <si>
+    <t>Coffee, Arabica</t>
+  </si>
+  <si>
+    <t>Coffee, Robusta</t>
+  </si>
+  <si>
+    <t>Tea, avg 3 auctions</t>
+  </si>
+  <si>
+    <t>Groundnut oil</t>
+  </si>
+  <si>
+    <t>Soybeans</t>
+  </si>
+  <si>
+    <t>Wheat, US SRW</t>
+  </si>
+  <si>
+    <t>Fish meal</t>
+  </si>
+  <si>
+    <t>Beef</t>
+  </si>
+  <si>
+    <t>Meat, chicken</t>
+  </si>
+  <si>
+    <t>Sugar, world</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Urea </t>
+  </si>
+  <si>
+    <t>Aluminum</t>
+  </si>
+  <si>
+    <t>Tin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -552,8 +552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M60"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,31 +574,31 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="K1">
         <f t="shared" ref="K1:K32" si="0">COUNTIF($A$2:$I$18,L1)</f>
@@ -608,7 +608,7 @@
         <v>1</v>
       </c>
       <c r="M1" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -631,7 +631,7 @@
         <v>35</v>
       </c>
       <c r="G2" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H2" s="2">
         <v>47</v>
@@ -647,7 +647,7 @@
         <v>2</v>
       </c>
       <c r="M2" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -670,10 +670,10 @@
         <v>36</v>
       </c>
       <c r="G3" s="2">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H3" s="2">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I3" s="2">
         <v>55</v>
@@ -686,7 +686,7 @@
         <v>3</v>
       </c>
       <c r="M3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -708,29 +708,27 @@
       <c r="F4" s="2">
         <v>37</v>
       </c>
-      <c r="G4" s="2">
-        <v>44</v>
-      </c>
+      <c r="G4" s="2"/>
       <c r="H4" s="2">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I4" s="2">
         <v>56</v>
       </c>
       <c r="K4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L4" s="1">
         <v>4</v>
       </c>
       <c r="M4" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2">
         <v>11</v>
@@ -747,11 +745,8 @@
       <c r="F5" s="2">
         <v>38</v>
       </c>
-      <c r="G5" s="2">
-        <v>45</v>
-      </c>
       <c r="H5" s="2">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I5" s="2"/>
       <c r="K5">
@@ -762,19 +757,19 @@
         <v>5</v>
       </c>
       <c r="M5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2">
         <v>16</v>
       </c>
       <c r="D6" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E6" s="2">
         <v>31</v>
@@ -782,11 +777,9 @@
       <c r="F6" s="2">
         <v>39</v>
       </c>
-      <c r="G6" s="2">
-        <v>46</v>
-      </c>
+      <c r="G6" s="2"/>
       <c r="H6" s="2">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I6" s="2"/>
       <c r="K6">
@@ -797,20 +790,14 @@
         <v>6</v>
       </c>
       <c r="M6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>6</v>
-      </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2">
         <v>17</v>
       </c>
-      <c r="D7" s="2">
-        <v>26</v>
-      </c>
       <c r="E7" s="2">
         <v>32</v>
       </c>
@@ -819,24 +806,22 @@
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I7" s="2"/>
       <c r="K7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L7" s="1">
         <v>7</v>
       </c>
       <c r="M7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>7</v>
-      </c>
+      <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2">
         <v>18</v>
@@ -845,13 +830,9 @@
       <c r="E8" s="2">
         <v>33</v>
       </c>
-      <c r="F8" s="2">
-        <v>41</v>
-      </c>
+      <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="2">
-        <v>53</v>
-      </c>
+      <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="K8">
         <f t="shared" si="0"/>
@@ -861,22 +842,19 @@
         <v>8</v>
       </c>
       <c r="M8" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
-      <c r="C9" s="2">
-        <v>19</v>
-      </c>
+      <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2">
         <v>34</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="K9">
         <f t="shared" si="0"/>
@@ -886,15 +864,13 @@
         <v>9</v>
       </c>
       <c r="M9" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
-      <c r="C10" s="2">
-        <v>20</v>
-      </c>
+      <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -909,7 +885,7 @@
         <v>10</v>
       </c>
       <c r="M10" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -930,7 +906,7 @@
         <v>11</v>
       </c>
       <c r="M11" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -951,7 +927,7 @@
         <v>12</v>
       </c>
       <c r="M12" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -972,7 +948,7 @@
         <v>13</v>
       </c>
       <c r="M13" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -993,7 +969,7 @@
         <v>14</v>
       </c>
       <c r="M14" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -1014,7 +990,7 @@
         <v>15</v>
       </c>
       <c r="M15" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -1035,7 +1011,7 @@
         <v>16</v>
       </c>
       <c r="M16" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -1056,7 +1032,7 @@
         <v>17</v>
       </c>
       <c r="M17" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -1077,7 +1053,7 @@
         <v>18</v>
       </c>
       <c r="M18" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -1092,13 +1068,13 @@
       <c r="I19" s="2"/>
       <c r="K19">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L19" s="1">
         <v>19</v>
       </c>
       <c r="M19" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -1113,13 +1089,13 @@
       <c r="I20" s="2"/>
       <c r="K20">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L20" s="1">
         <v>20</v>
       </c>
       <c r="M20" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -1140,7 +1116,7 @@
         <v>21</v>
       </c>
       <c r="M21" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -1161,7 +1137,7 @@
         <v>22</v>
       </c>
       <c r="M22" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -1173,7 +1149,7 @@
         <v>23</v>
       </c>
       <c r="M23" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -1185,19 +1161,19 @@
         <v>24</v>
       </c>
       <c r="M24" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L25" s="1">
         <v>25</v>
       </c>
       <c r="M25" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -1209,7 +1185,7 @@
         <v>26</v>
       </c>
       <c r="M26" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
@@ -1221,7 +1197,7 @@
         <v>27</v>
       </c>
       <c r="M27" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
@@ -1233,7 +1209,7 @@
         <v>28</v>
       </c>
       <c r="M28" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
@@ -1245,7 +1221,7 @@
         <v>29</v>
       </c>
       <c r="M29" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -1257,7 +1233,7 @@
         <v>30</v>
       </c>
       <c r="M30" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -1269,7 +1245,7 @@
         <v>31</v>
       </c>
       <c r="M31" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -1281,19 +1257,19 @@
         <v>32</v>
       </c>
       <c r="M32" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K33">
-        <f t="shared" ref="K33:K64" si="1">COUNTIF($A$2:$I$18,L33)</f>
+        <f t="shared" ref="K33:K60" si="1">COUNTIF($A$2:$I$18,L33)</f>
         <v>1</v>
       </c>
       <c r="L33" s="1">
         <v>33</v>
       </c>
       <c r="M33" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="11:13" x14ac:dyDescent="0.25">
@@ -1305,7 +1281,7 @@
         <v>34</v>
       </c>
       <c r="M34" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="11:13" x14ac:dyDescent="0.25">
@@ -1317,7 +1293,7 @@
         <v>35</v>
       </c>
       <c r="M35" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36" spans="11:13" x14ac:dyDescent="0.25">
@@ -1329,7 +1305,7 @@
         <v>36</v>
       </c>
       <c r="M36" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="11:13" x14ac:dyDescent="0.25">
@@ -1341,7 +1317,7 @@
         <v>37</v>
       </c>
       <c r="M37" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38" spans="11:13" x14ac:dyDescent="0.25">
@@ -1353,7 +1329,7 @@
         <v>38</v>
       </c>
       <c r="M38" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39" spans="11:13" x14ac:dyDescent="0.25">
@@ -1365,7 +1341,7 @@
         <v>39</v>
       </c>
       <c r="M39" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="11:13" x14ac:dyDescent="0.25">
@@ -1377,31 +1353,31 @@
         <v>40</v>
       </c>
       <c r="M40" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K41">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L41" s="1">
         <v>41</v>
       </c>
       <c r="M41" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="42" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K42">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L42" s="1">
         <v>42</v>
       </c>
       <c r="M42" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="11:13" x14ac:dyDescent="0.25">
@@ -1413,19 +1389,19 @@
         <v>43</v>
       </c>
       <c r="M43" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="44" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K44">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L44" s="1">
         <v>44</v>
       </c>
       <c r="M44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="11:13" x14ac:dyDescent="0.25">
@@ -1437,19 +1413,19 @@
         <v>45</v>
       </c>
       <c r="M45" t="s">
-        <v>11</v>
+        <v>62</v>
       </c>
     </row>
     <row r="46" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K46">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L46" s="1">
         <v>46</v>
       </c>
       <c r="M46" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47" spans="11:13" x14ac:dyDescent="0.25">
@@ -1461,19 +1437,19 @@
         <v>47</v>
       </c>
       <c r="M47" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
     </row>
     <row r="48" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K48">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L48" s="1">
         <v>48</v>
       </c>
       <c r="M48" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49" spans="11:13" x14ac:dyDescent="0.25">
@@ -1485,7 +1461,7 @@
         <v>49</v>
       </c>
       <c r="M49" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="11:13" x14ac:dyDescent="0.25">
@@ -1497,7 +1473,7 @@
         <v>50</v>
       </c>
       <c r="M50" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="11:13" x14ac:dyDescent="0.25">
@@ -1509,7 +1485,7 @@
         <v>51</v>
       </c>
       <c r="M51" t="s">
-        <v>5</v>
+        <v>64</v>
       </c>
     </row>
     <row r="52" spans="11:13" x14ac:dyDescent="0.25">
@@ -1521,7 +1497,7 @@
         <v>52</v>
       </c>
       <c r="M52" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53" spans="11:13" x14ac:dyDescent="0.25">
@@ -1533,7 +1509,7 @@
         <v>53</v>
       </c>
       <c r="M53" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54" spans="11:13" x14ac:dyDescent="0.25">
@@ -1545,7 +1521,7 @@
         <v>54</v>
       </c>
       <c r="M54" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="11:13" x14ac:dyDescent="0.25">
@@ -1557,7 +1533,7 @@
         <v>55</v>
       </c>
       <c r="M55" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="11:13" x14ac:dyDescent="0.25">
@@ -1569,7 +1545,7 @@
         <v>56</v>
       </c>
       <c r="M56" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="11:13" x14ac:dyDescent="0.25">
@@ -1629,7 +1605,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -1641,10 +1617,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Create block example excel
</commit_message>
<xml_diff>
--- a/Block_WBC.xlsx
+++ b/Block_WBC.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="B1" sheetId="1" r:id="rId1"/>
-    <sheet name="B2" sheetId="2" r:id="rId2"/>
+    <sheet name="Flexi" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="67">
   <si>
     <t>Platinum</t>
   </si>
@@ -220,6 +220,12 @@
   </si>
   <si>
     <t>Tin</t>
+  </si>
+  <si>
+    <t>Nutrients</t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
 </sst>
 </file>
@@ -241,18 +247,33 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -261,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -270,12 +291,112 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF7C80"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -552,8 +673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:M60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,7 +829,9 @@
       <c r="F4" s="2">
         <v>37</v>
       </c>
-      <c r="G4" s="2"/>
+      <c r="G4" s="2">
+        <v>41</v>
+      </c>
       <c r="H4" s="2">
         <v>50</v>
       </c>
@@ -717,7 +840,7 @@
       </c>
       <c r="K4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4" s="1">
         <v>4</v>
@@ -745,6 +868,9 @@
       <c r="F5" s="2">
         <v>38</v>
       </c>
+      <c r="G5" s="2">
+        <v>42</v>
+      </c>
       <c r="H5" s="2">
         <v>51</v>
       </c>
@@ -777,7 +903,9 @@
       <c r="F6" s="2">
         <v>39</v>
       </c>
-      <c r="G6" s="2"/>
+      <c r="G6" s="2">
+        <v>44</v>
+      </c>
       <c r="H6" s="2">
         <v>52</v>
       </c>
@@ -794,24 +922,32 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>4</v>
+      </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2">
         <v>17</v>
       </c>
+      <c r="D7" s="2">
+        <v>25</v>
+      </c>
       <c r="E7" s="2">
         <v>32</v>
       </c>
       <c r="F7" s="2">
         <v>40</v>
       </c>
-      <c r="G7" s="2"/>
+      <c r="G7" s="2">
+        <v>46</v>
+      </c>
       <c r="H7" s="2">
         <v>53</v>
       </c>
       <c r="I7" s="2"/>
       <c r="K7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L7" s="1">
         <v>7</v>
@@ -821,7 +957,9 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2">
         <v>18</v>
@@ -832,7 +970,9 @@
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="H8" s="2">
+        <v>48</v>
+      </c>
       <c r="I8" s="2"/>
       <c r="K8">
         <f t="shared" si="0"/>
@@ -848,7 +988,9 @@
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="C9" s="2">
+        <v>19</v>
+      </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2">
         <v>34</v>
@@ -870,7 +1012,9 @@
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
+      <c r="C10" s="2">
+        <v>20</v>
+      </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -1068,7 +1212,7 @@
       <c r="I19" s="2"/>
       <c r="K19">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L19" s="1">
         <v>19</v>
@@ -1089,7 +1233,7 @@
       <c r="I20" s="2"/>
       <c r="K20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L20" s="1">
         <v>20</v>
@@ -1167,7 +1311,7 @@
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L25" s="1">
         <v>25</v>
@@ -1359,7 +1503,7 @@
     <row r="41" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K41">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L41" s="1">
         <v>41</v>
@@ -1371,7 +1515,7 @@
     <row r="42" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K42">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L42" s="1">
         <v>42</v>
@@ -1395,7 +1539,7 @@
     <row r="44" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K44">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L44" s="1">
         <v>44</v>
@@ -1419,7 +1563,7 @@
     <row r="46" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K46">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L46" s="1">
         <v>46</v>
@@ -1443,7 +1587,7 @@
     <row r="48" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K48">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L48" s="1">
         <v>48</v>
@@ -1603,43 +1747,1155 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:O60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.140625" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="3" max="3" width="3.140625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="4" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="4">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="6">
+        <f>COUNTIF($E$2:$AH$61, A1)</f>
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2">
+      <c r="J1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="6">
+        <f>COUNTIF($E$2:$AH$61, A2)</f>
+        <v>2</v>
+      </c>
+      <c r="E2" s="2">
+        <v>8</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2">
+        <v>8</v>
+      </c>
+      <c r="I2" s="2">
+        <v>12</v>
+      </c>
+      <c r="J2" s="2">
+        <v>21</v>
+      </c>
+      <c r="K2" s="2">
+        <v>27</v>
+      </c>
+      <c r="L2" s="2">
+        <v>35</v>
+      </c>
+      <c r="M2" s="2">
+        <v>43</v>
+      </c>
+      <c r="N2" s="2">
+        <v>47</v>
+      </c>
+      <c r="O2" s="2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2">
+      <c r="B3" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="6">
+        <f t="shared" ref="C3:C60" si="0">COUNTIF($E$2:$AH$61, A3)</f>
+        <v>2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>9</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2">
+        <v>2</v>
+      </c>
+      <c r="H3" s="2">
+        <v>9</v>
+      </c>
+      <c r="I3" s="2">
+        <v>13</v>
+      </c>
+      <c r="J3" s="2">
+        <v>22</v>
+      </c>
+      <c r="K3" s="2">
+        <v>28</v>
+      </c>
+      <c r="L3" s="2">
+        <v>36</v>
+      </c>
+      <c r="M3" s="2">
+        <v>45</v>
+      </c>
+      <c r="N3" s="2">
+        <v>49</v>
+      </c>
+      <c r="O3" s="2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
         <v>4</v>
       </c>
+      <c r="B4" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>10</v>
+      </c>
+      <c r="F4" s="2">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2">
+        <v>3</v>
+      </c>
+      <c r="H4" s="2">
+        <v>10</v>
+      </c>
+      <c r="I4" s="2">
+        <v>14</v>
+      </c>
+      <c r="J4" s="2">
+        <v>23</v>
+      </c>
+      <c r="K4" s="2">
+        <v>29</v>
+      </c>
+      <c r="L4" s="2">
+        <v>37</v>
+      </c>
+      <c r="M4" s="2">
+        <v>41</v>
+      </c>
+      <c r="N4" s="2">
+        <v>50</v>
+      </c>
+      <c r="O4" s="2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>5</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>11</v>
+      </c>
+      <c r="F5" s="2">
+        <v>5</v>
+      </c>
+      <c r="G5" s="2">
+        <v>5</v>
+      </c>
+      <c r="H5" s="2">
+        <v>11</v>
+      </c>
+      <c r="I5" s="2">
+        <v>15</v>
+      </c>
+      <c r="J5" s="2">
+        <v>24</v>
+      </c>
+      <c r="K5" s="2">
+        <v>30</v>
+      </c>
+      <c r="L5" s="2">
+        <v>38</v>
+      </c>
+      <c r="M5" s="2">
+        <v>42</v>
+      </c>
+      <c r="N5" s="2">
+        <v>51</v>
+      </c>
+      <c r="O5" s="2"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>6</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E6" s="2">
+        <v>12</v>
+      </c>
+      <c r="F6" s="2">
+        <v>6</v>
+      </c>
+      <c r="G6" s="2">
+        <v>6</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2">
+        <v>16</v>
+      </c>
+      <c r="J6" s="2">
+        <v>26</v>
+      </c>
+      <c r="K6" s="2">
+        <v>31</v>
+      </c>
+      <c r="L6" s="2">
+        <v>39</v>
+      </c>
+      <c r="M6" s="2">
+        <v>44</v>
+      </c>
+      <c r="N6" s="2">
+        <v>52</v>
+      </c>
+      <c r="O6" s="2"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>7</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>13</v>
+      </c>
+      <c r="F7" s="2">
+        <v>4</v>
+      </c>
+      <c r="G7" s="2">
+        <v>4</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2">
+        <v>17</v>
+      </c>
+      <c r="J7" s="2">
+        <v>25</v>
+      </c>
+      <c r="K7" s="2">
+        <v>32</v>
+      </c>
+      <c r="L7" s="2">
+        <v>40</v>
+      </c>
+      <c r="M7" s="2">
+        <v>46</v>
+      </c>
+      <c r="N7" s="2">
+        <v>53</v>
+      </c>
+      <c r="O7" s="2"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>8</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E8" s="2">
+        <v>14</v>
+      </c>
+      <c r="F8" s="2">
+        <v>7</v>
+      </c>
+      <c r="G8" s="2">
+        <v>7</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2">
+        <v>18</v>
+      </c>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2">
+        <v>33</v>
+      </c>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2">
+        <v>48</v>
+      </c>
+      <c r="O8" s="2"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>9</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E9" s="2">
+        <v>15</v>
+      </c>
+      <c r="F9" s="2">
+        <v>35</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2">
+        <v>19</v>
+      </c>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2">
+        <v>34</v>
+      </c>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="O9" s="2"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>10</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E10" s="2">
+        <v>16</v>
+      </c>
+      <c r="F10" s="2">
+        <v>36</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2">
+        <v>20</v>
+      </c>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>11</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E11" s="2">
+        <v>17</v>
+      </c>
+      <c r="F11" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>12</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E12" s="2">
+        <v>18</v>
+      </c>
+      <c r="F12" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>13</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E13" s="2">
+        <v>19</v>
+      </c>
+      <c r="F13" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>14</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E14" s="2">
+        <v>20</v>
+      </c>
+      <c r="F14" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>15</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E15" s="2">
+        <v>21</v>
+      </c>
+      <c r="F15" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>16</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E16" s="2">
+        <v>22</v>
+      </c>
+      <c r="F16" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>17</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E17" s="2">
+        <v>23</v>
+      </c>
+      <c r="F17" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>18</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E18" s="2">
+        <v>24</v>
+      </c>
+      <c r="F18" s="2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>19</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E19" s="2">
+        <v>26</v>
+      </c>
+      <c r="F19" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>20</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E20" s="2">
+        <v>25</v>
+      </c>
+      <c r="F20" s="2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>21</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E21" s="2">
+        <v>27</v>
+      </c>
+      <c r="F21" s="2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>22</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E22" s="2">
+        <v>28</v>
+      </c>
+      <c r="F22" s="2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>23</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E23" s="2">
+        <v>29</v>
+      </c>
+      <c r="F23" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>24</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E24" s="2">
+        <v>30</v>
+      </c>
+      <c r="F24" s="2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>25</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E25" s="2">
+        <v>31</v>
+      </c>
+      <c r="F25" s="2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>26</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E26" s="2">
+        <v>32</v>
+      </c>
+      <c r="F26" s="2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>27</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E27" s="2">
+        <v>33</v>
+      </c>
+      <c r="F27" s="2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>28</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E28" s="2">
+        <v>34</v>
+      </c>
+      <c r="F28" s="2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>29</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F29" s="2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>30</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F30" s="2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>31</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>32</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>33</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>34</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>35</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>36</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>37</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>38</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <v>39</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
+        <v>40</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
+        <v>41</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
+        <v>42</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="4">
+        <v>43</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
+        <v>44</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="4">
+        <v>45</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C45" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="4">
+        <v>46</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
+        <v>47</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C47" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="4">
+        <v>48</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C48" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="4">
+        <v>49</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C49" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="4">
+        <v>50</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="4">
+        <v>51</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C51" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="4">
+        <v>52</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C52" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="4">
+        <v>53</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="4">
+        <v>54</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C54" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="4">
+        <v>55</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C55" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="4">
+        <v>56</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C56" s="6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="4">
+        <v>57</v>
+      </c>
+      <c r="B57" s="5"/>
+      <c r="C57" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="4">
+        <v>58</v>
+      </c>
+      <c r="B58" s="5"/>
+      <c r="C58" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="4">
+        <v>59</v>
+      </c>
+      <c r="B59" s="5"/>
+      <c r="C59" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="4">
+        <v>60</v>
+      </c>
+      <c r="B60" s="5"/>
+      <c r="C60" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:C60">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$C1=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add possibility of flexible block structure
</commit_message>
<xml_diff>
--- a/Block_WBC.xlsx
+++ b/Block_WBC.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="B1" sheetId="1" r:id="rId1"/>
@@ -299,7 +299,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="2">
     <dxf>
       <font>
         <color theme="0"/>
@@ -317,96 +317,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -693,7 +603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
@@ -1867,8 +1777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O60"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection sqref="A1:C60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1879,11 +1789,11 @@
     <col min="4" max="4" width="4" customWidth="1"/>
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7.5703125" bestFit="1" customWidth="1"/>
@@ -1907,20 +1817,20 @@
       <c r="F1" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>38</v>
@@ -1953,19 +1863,19 @@
         <v>1</v>
       </c>
       <c r="G2" s="2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H2" s="2">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I2" s="2">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="J2" s="2">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="K2" s="2">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="L2" s="2">
         <v>35</v>
@@ -1988,7 +1898,7 @@
         <v>46</v>
       </c>
       <c r="C3" s="6">
-        <f t="shared" ref="C3:C60" si="0">COUNTIF($E$2:$AH$61, A3)</f>
+        <f>COUNTIF($E$2:$AH$61, A3)</f>
         <v>2</v>
       </c>
       <c r="E3" s="2">
@@ -1998,19 +1908,19 @@
         <v>2</v>
       </c>
       <c r="G3" s="2">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="H3" s="2">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="I3" s="2">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="J3" s="2">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="K3" s="2">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="L3" s="2">
         <v>36</v>
@@ -2033,7 +1943,7 @@
         <v>47</v>
       </c>
       <c r="C4" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A4)</f>
         <v>2</v>
       </c>
       <c r="E4" s="2">
@@ -2043,19 +1953,19 @@
         <v>3</v>
       </c>
       <c r="G4" s="2">
+        <v>10</v>
+      </c>
+      <c r="H4" s="2">
+        <v>14</v>
+      </c>
+      <c r="I4" s="2">
+        <v>23</v>
+      </c>
+      <c r="J4" s="2">
+        <v>29</v>
+      </c>
+      <c r="K4" s="2">
         <v>3</v>
-      </c>
-      <c r="H4" s="2">
-        <v>10</v>
-      </c>
-      <c r="I4" s="2">
-        <v>14</v>
-      </c>
-      <c r="J4" s="2">
-        <v>23</v>
-      </c>
-      <c r="K4" s="2">
-        <v>29</v>
       </c>
       <c r="L4" s="2">
         <v>37</v>
@@ -2078,7 +1988,7 @@
         <v>48</v>
       </c>
       <c r="C5" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A5)</f>
         <v>2</v>
       </c>
       <c r="E5" s="2">
@@ -2088,19 +1998,19 @@
         <v>5</v>
       </c>
       <c r="G5" s="2">
+        <v>11</v>
+      </c>
+      <c r="H5" s="2">
+        <v>15</v>
+      </c>
+      <c r="I5" s="2">
+        <v>24</v>
+      </c>
+      <c r="J5" s="2">
+        <v>30</v>
+      </c>
+      <c r="K5" s="2">
         <v>5</v>
-      </c>
-      <c r="H5" s="2">
-        <v>11</v>
-      </c>
-      <c r="I5" s="2">
-        <v>15</v>
-      </c>
-      <c r="J5" s="2">
-        <v>24</v>
-      </c>
-      <c r="K5" s="2">
-        <v>30</v>
       </c>
       <c r="L5" s="2">
         <v>38</v>
@@ -2121,7 +2031,7 @@
         <v>49</v>
       </c>
       <c r="C6" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A6)</f>
         <v>2</v>
       </c>
       <c r="E6" s="2">
@@ -2130,18 +2040,18 @@
       <c r="F6" s="2">
         <v>6</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="2"/>
+      <c r="H6" s="2">
+        <v>16</v>
+      </c>
+      <c r="I6" s="2">
+        <v>26</v>
+      </c>
+      <c r="J6" s="2">
+        <v>31</v>
+      </c>
+      <c r="K6" s="2">
         <v>6</v>
-      </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2">
-        <v>16</v>
-      </c>
-      <c r="J6" s="2">
-        <v>26</v>
-      </c>
-      <c r="K6" s="2">
-        <v>31</v>
       </c>
       <c r="L6" s="2">
         <v>39</v>
@@ -2162,7 +2072,7 @@
         <v>50</v>
       </c>
       <c r="C7" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A7)</f>
         <v>2</v>
       </c>
       <c r="E7" s="2">
@@ -2171,18 +2081,18 @@
       <c r="F7" s="2">
         <v>4</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="2"/>
+      <c r="H7" s="2">
+        <v>17</v>
+      </c>
+      <c r="I7" s="2">
+        <v>25</v>
+      </c>
+      <c r="J7" s="2">
+        <v>32</v>
+      </c>
+      <c r="K7" s="2">
         <v>4</v>
-      </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2">
-        <v>17</v>
-      </c>
-      <c r="J7" s="2">
-        <v>25</v>
-      </c>
-      <c r="K7" s="2">
-        <v>32</v>
       </c>
       <c r="L7" s="2">
         <v>40</v>
@@ -2203,7 +2113,7 @@
         <v>51</v>
       </c>
       <c r="C8" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A8)</f>
         <v>2</v>
       </c>
       <c r="E8" s="2">
@@ -2212,16 +2122,16 @@
       <c r="F8" s="2">
         <v>7</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="2"/>
+      <c r="H8" s="2">
+        <v>18</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2">
+        <v>33</v>
+      </c>
+      <c r="K8" s="2">
         <v>7</v>
-      </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2">
-        <v>18</v>
-      </c>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2">
-        <v>33</v>
       </c>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -2238,7 +2148,7 @@
         <v>52</v>
       </c>
       <c r="C9" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A9)</f>
         <v>2</v>
       </c>
       <c r="E9" s="2">
@@ -2248,14 +2158,14 @@
         <v>35</v>
       </c>
       <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2">
+      <c r="H9" s="2">
         <v>19</v>
       </c>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2">
+      <c r="I9" s="2"/>
+      <c r="J9" s="2">
         <v>34</v>
       </c>
+      <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="O9" s="2"/>
@@ -2268,7 +2178,7 @@
         <v>53</v>
       </c>
       <c r="C10" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A10)</f>
         <v>2</v>
       </c>
       <c r="E10" s="2">
@@ -2278,10 +2188,10 @@
         <v>36</v>
       </c>
       <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2">
+      <c r="H10" s="2">
         <v>20</v>
       </c>
+      <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
@@ -2297,7 +2207,7 @@
         <v>54</v>
       </c>
       <c r="C11" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A11)</f>
         <v>2</v>
       </c>
       <c r="E11" s="2">
@@ -2315,7 +2225,7 @@
         <v>34</v>
       </c>
       <c r="C12" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A12)</f>
         <v>2</v>
       </c>
       <c r="E12" s="2">
@@ -2333,7 +2243,7 @@
         <v>33</v>
       </c>
       <c r="C13" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A13)</f>
         <v>2</v>
       </c>
       <c r="E13" s="2">
@@ -2351,7 +2261,7 @@
         <v>32</v>
       </c>
       <c r="C14" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A14)</f>
         <v>2</v>
       </c>
       <c r="E14" s="2">
@@ -2369,7 +2279,7 @@
         <v>55</v>
       </c>
       <c r="C15" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A15)</f>
         <v>2</v>
       </c>
       <c r="E15" s="2">
@@ -2387,7 +2297,7 @@
         <v>31</v>
       </c>
       <c r="C16" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A16)</f>
         <v>2</v>
       </c>
       <c r="E16" s="2">
@@ -2405,7 +2315,7 @@
         <v>56</v>
       </c>
       <c r="C17" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A17)</f>
         <v>2</v>
       </c>
       <c r="E17" s="2">
@@ -2423,7 +2333,7 @@
         <v>30</v>
       </c>
       <c r="C18" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A18)</f>
         <v>2</v>
       </c>
       <c r="E18" s="2">
@@ -2441,7 +2351,7 @@
         <v>29</v>
       </c>
       <c r="C19" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A19)</f>
         <v>2</v>
       </c>
       <c r="E19" s="2">
@@ -2459,7 +2369,7 @@
         <v>28</v>
       </c>
       <c r="C20" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A20)</f>
         <v>2</v>
       </c>
       <c r="E20" s="2">
@@ -2477,7 +2387,7 @@
         <v>27</v>
       </c>
       <c r="C21" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A21)</f>
         <v>2</v>
       </c>
       <c r="E21" s="2">
@@ -2495,7 +2405,7 @@
         <v>26</v>
       </c>
       <c r="C22" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A22)</f>
         <v>2</v>
       </c>
       <c r="E22" s="2">
@@ -2513,7 +2423,7 @@
         <v>23</v>
       </c>
       <c r="C23" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A23)</f>
         <v>2</v>
       </c>
       <c r="E23" s="2">
@@ -2531,7 +2441,7 @@
         <v>25</v>
       </c>
       <c r="C24" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A24)</f>
         <v>2</v>
       </c>
       <c r="E24" s="2">
@@ -2549,7 +2459,7 @@
         <v>24</v>
       </c>
       <c r="C25" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A25)</f>
         <v>2</v>
       </c>
       <c r="E25" s="2">
@@ -2567,7 +2477,7 @@
         <v>57</v>
       </c>
       <c r="C26" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A26)</f>
         <v>2</v>
       </c>
       <c r="E26" s="2">
@@ -2585,7 +2495,7 @@
         <v>22</v>
       </c>
       <c r="C27" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A27)</f>
         <v>2</v>
       </c>
       <c r="E27" s="2">
@@ -2603,7 +2513,7 @@
         <v>19</v>
       </c>
       <c r="C28" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A28)</f>
         <v>2</v>
       </c>
       <c r="E28" s="2">
@@ -2621,7 +2531,7 @@
         <v>58</v>
       </c>
       <c r="C29" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A29)</f>
         <v>2</v>
       </c>
       <c r="F29" s="2">
@@ -2636,7 +2546,7 @@
         <v>59</v>
       </c>
       <c r="C30" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A30)</f>
         <v>2</v>
       </c>
       <c r="F30" s="2">
@@ -2651,7 +2561,7 @@
         <v>60</v>
       </c>
       <c r="C31" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A31)</f>
         <v>2</v>
       </c>
     </row>
@@ -2663,7 +2573,7 @@
         <v>21</v>
       </c>
       <c r="C32" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A32)</f>
         <v>2</v>
       </c>
     </row>
@@ -2675,7 +2585,7 @@
         <v>20</v>
       </c>
       <c r="C33" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A33)</f>
         <v>2</v>
       </c>
     </row>
@@ -2687,7 +2597,7 @@
         <v>61</v>
       </c>
       <c r="C34" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A34)</f>
         <v>2</v>
       </c>
     </row>
@@ -2699,7 +2609,7 @@
         <v>18</v>
       </c>
       <c r="C35" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A35)</f>
         <v>2</v>
       </c>
     </row>
@@ -2711,7 +2621,7 @@
         <v>17</v>
       </c>
       <c r="C36" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A36)</f>
         <v>2</v>
       </c>
     </row>
@@ -2723,7 +2633,7 @@
         <v>16</v>
       </c>
       <c r="C37" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A37)</f>
         <v>2</v>
       </c>
     </row>
@@ -2735,7 +2645,7 @@
         <v>15</v>
       </c>
       <c r="C38" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A38)</f>
         <v>2</v>
       </c>
     </row>
@@ -2747,7 +2657,7 @@
         <v>14</v>
       </c>
       <c r="C39" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A39)</f>
         <v>2</v>
       </c>
     </row>
@@ -2759,7 +2669,7 @@
         <v>12</v>
       </c>
       <c r="C40" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A40)</f>
         <v>2</v>
       </c>
     </row>
@@ -2771,7 +2681,7 @@
         <v>13</v>
       </c>
       <c r="C41" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A41)</f>
         <v>2</v>
       </c>
     </row>
@@ -2783,7 +2693,7 @@
         <v>8</v>
       </c>
       <c r="C42" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A42)</f>
         <v>2</v>
       </c>
     </row>
@@ -2795,7 +2705,7 @@
         <v>11</v>
       </c>
       <c r="C43" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A43)</f>
         <v>2</v>
       </c>
     </row>
@@ -2807,7 +2717,7 @@
         <v>10</v>
       </c>
       <c r="C44" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A44)</f>
         <v>2</v>
       </c>
     </row>
@@ -2819,7 +2729,7 @@
         <v>62</v>
       </c>
       <c r="C45" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A45)</f>
         <v>2</v>
       </c>
     </row>
@@ -2831,7 +2741,7 @@
         <v>9</v>
       </c>
       <c r="C46" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A46)</f>
         <v>2</v>
       </c>
     </row>
@@ -2843,7 +2753,7 @@
         <v>63</v>
       </c>
       <c r="C47" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A47)</f>
         <v>2</v>
       </c>
     </row>
@@ -2855,7 +2765,7 @@
         <v>7</v>
       </c>
       <c r="C48" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A48)</f>
         <v>2</v>
       </c>
     </row>
@@ -2867,7 +2777,7 @@
         <v>4</v>
       </c>
       <c r="C49" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A49)</f>
         <v>2</v>
       </c>
     </row>
@@ -2879,7 +2789,7 @@
         <v>5</v>
       </c>
       <c r="C50" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A50)</f>
         <v>2</v>
       </c>
     </row>
@@ -2891,7 +2801,7 @@
         <v>64</v>
       </c>
       <c r="C51" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A51)</f>
         <v>2</v>
       </c>
     </row>
@@ -2903,7 +2813,7 @@
         <v>3</v>
       </c>
       <c r="C52" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A52)</f>
         <v>2</v>
       </c>
     </row>
@@ -2915,7 +2825,7 @@
         <v>6</v>
       </c>
       <c r="C53" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A53)</f>
         <v>2</v>
       </c>
     </row>
@@ -2927,7 +2837,7 @@
         <v>1</v>
       </c>
       <c r="C54" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A54)</f>
         <v>2</v>
       </c>
     </row>
@@ -2939,7 +2849,7 @@
         <v>0</v>
       </c>
       <c r="C55" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A55)</f>
         <v>2</v>
       </c>
     </row>
@@ -2951,7 +2861,7 @@
         <v>2</v>
       </c>
       <c r="C56" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A56)</f>
         <v>2</v>
       </c>
     </row>
@@ -2961,7 +2871,7 @@
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A57)</f>
         <v>0</v>
       </c>
     </row>
@@ -2971,7 +2881,7 @@
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A58)</f>
         <v>0</v>
       </c>
     </row>
@@ -2981,7 +2891,7 @@
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A59)</f>
         <v>0</v>
       </c>
     </row>
@@ -2991,7 +2901,7 @@
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="6">
-        <f t="shared" si="0"/>
+        <f>COUNTIF($E$2:$AH$61, A60)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implement fully flexible A matrix with possibility of lags larger than 1
</commit_message>
<xml_diff>
--- a/Block_WBC.xlsx
+++ b/Block_WBC.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sigvekb\Master\dynamic-factor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sigve Borgmo\OneDrive - NTNU\Indok\Master\dynamic-factor\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E35C3127-1947-4155-9B78-48530E6DFBFE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="B1" sheetId="1" r:id="rId1"/>
     <sheet name="Flexi" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="72">
   <si>
     <t>Platinum</t>
   </si>
@@ -226,13 +227,28 @@
   </si>
   <si>
     <t>Other</t>
+  </si>
+  <si>
+    <t>Global</t>
+  </si>
+  <si>
+    <t>Lags in VAR</t>
+  </si>
+  <si>
+    <t>Variables</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>bv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,6 +257,12 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -261,7 +283,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -278,11 +300,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -295,6 +328,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -600,26 +648,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O60"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="K5" sqref="K5:K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.5703125" customWidth="1"/>
-    <col min="4" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.5546875" customWidth="1"/>
+    <col min="4" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.5546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1774,33 +1822,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O60"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:Q60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.140625" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" customWidth="1"/>
-    <col min="3" max="3" width="3.140625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="4.109375" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" customWidth="1"/>
+    <col min="3" max="3" width="3.109375" style="7" customWidth="1"/>
     <col min="4" max="4" width="4" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" customWidth="1"/>
+    <col min="6" max="6" width="7.77734375" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" customWidth="1"/>
+    <col min="8" max="8" width="7.21875" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" customWidth="1"/>
+    <col min="10" max="10" width="13.109375" customWidth="1"/>
+    <col min="11" max="11" width="8.5546875" customWidth="1"/>
+    <col min="12" max="12" width="11.88671875" customWidth="1"/>
+    <col min="13" max="13" width="8.77734375" customWidth="1"/>
+    <col min="14" max="14" width="14.6640625" customWidth="1"/>
+    <col min="15" max="15" width="10.5546875" customWidth="1"/>
+    <col min="16" max="16" width="8" customWidth="1"/>
+    <col min="17" max="17" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="4">
         <v>1</v>
       </c>
@@ -1808,44 +1858,48 @@
         <v>44</v>
       </c>
       <c r="C1" s="6">
-        <f>COUNTIF($E$2:$AH$61, A1)</f>
-        <v>2</v>
-      </c>
-      <c r="E1" s="3" t="s">
+        <f>COUNTIF($G$3:$AI$100, A1)</f>
+        <v>2</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="Q1" s="8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>2</v>
       </c>
@@ -1853,44 +1907,50 @@
         <v>45</v>
       </c>
       <c r="C2" s="6">
-        <f>COUNTIF($E$2:$AH$61, A2)</f>
-        <v>2</v>
-      </c>
-      <c r="E2" s="2">
-        <v>8</v>
-      </c>
-      <c r="F2" s="2">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2">
-        <v>8</v>
-      </c>
-      <c r="H2" s="2">
-        <v>12</v>
-      </c>
-      <c r="I2" s="2">
-        <v>21</v>
-      </c>
-      <c r="J2" s="2">
-        <v>27</v>
-      </c>
-      <c r="K2" s="2">
-        <v>1</v>
-      </c>
-      <c r="L2" s="2">
-        <v>35</v>
-      </c>
-      <c r="M2" s="2">
-        <v>43</v>
-      </c>
-      <c r="N2" s="2">
-        <v>47</v>
-      </c>
-      <c r="O2" s="2">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" ref="C2:C60" si="0">COUNTIF($G$3:$AI$100, A2)</f>
+        <v>2</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="10">
+        <v>1</v>
+      </c>
+      <c r="G2" s="10">
+        <v>1</v>
+      </c>
+      <c r="H2" s="10">
+        <v>1</v>
+      </c>
+      <c r="I2" s="10">
+        <v>1</v>
+      </c>
+      <c r="J2" s="10">
+        <v>1</v>
+      </c>
+      <c r="K2" s="10">
+        <v>1</v>
+      </c>
+      <c r="L2" s="10">
+        <v>1</v>
+      </c>
+      <c r="M2" s="10">
+        <v>1</v>
+      </c>
+      <c r="N2" s="10">
+        <v>1</v>
+      </c>
+      <c r="O2" s="10">
+        <v>1</v>
+      </c>
+      <c r="P2" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>3</v>
       </c>
@@ -1898,44 +1958,50 @@
         <v>46</v>
       </c>
       <c r="C3" s="6">
-        <f>COUNTIF($E$2:$AH$61, A3)</f>
-        <v>2</v>
-      </c>
-      <c r="E3" s="2">
-        <v>9</v>
-      </c>
-      <c r="F3" s="2">
-        <v>2</v>
-      </c>
-      <c r="G3" s="2">
-        <v>9</v>
-      </c>
-      <c r="H3" s="2">
-        <v>13</v>
-      </c>
-      <c r="I3" s="2">
-        <v>22</v>
-      </c>
-      <c r="J3" s="2">
-        <v>28</v>
-      </c>
-      <c r="K3" s="2">
-        <v>2</v>
-      </c>
-      <c r="L3" s="2">
-        <v>36</v>
-      </c>
-      <c r="M3" s="2">
-        <v>45</v>
-      </c>
-      <c r="N3" s="2">
-        <v>49</v>
-      </c>
-      <c r="O3" s="2">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" s="12">
+        <v>8</v>
+      </c>
+      <c r="H3" s="12">
+        <v>1</v>
+      </c>
+      <c r="I3" s="12">
+        <v>8</v>
+      </c>
+      <c r="J3" s="12">
+        <v>12</v>
+      </c>
+      <c r="K3" s="12">
+        <v>21</v>
+      </c>
+      <c r="L3" s="12">
+        <v>27</v>
+      </c>
+      <c r="M3" s="12">
+        <v>1</v>
+      </c>
+      <c r="N3" s="12">
+        <v>35</v>
+      </c>
+      <c r="O3" s="12">
+        <v>43</v>
+      </c>
+      <c r="P3" s="12">
+        <v>47</v>
+      </c>
+      <c r="Q3" s="12">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>4</v>
       </c>
@@ -1943,44 +2009,46 @@
         <v>47</v>
       </c>
       <c r="C4" s="6">
-        <f>COUNTIF($E$2:$AH$61, A4)</f>
-        <v>2</v>
-      </c>
-      <c r="E4" s="2">
-        <v>10</v>
-      </c>
-      <c r="F4" s="2">
-        <v>3</v>
-      </c>
-      <c r="G4" s="2">
-        <v>10</v>
-      </c>
-      <c r="H4" s="2">
-        <v>14</v>
-      </c>
-      <c r="I4" s="2">
-        <v>23</v>
-      </c>
-      <c r="J4" s="2">
-        <v>29</v>
-      </c>
-      <c r="K4" s="2">
-        <v>3</v>
-      </c>
-      <c r="L4" s="2">
-        <v>37</v>
-      </c>
-      <c r="M4" s="2">
-        <v>41</v>
-      </c>
-      <c r="N4" s="2">
-        <v>50</v>
-      </c>
-      <c r="O4" s="2">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="12">
+        <v>9</v>
+      </c>
+      <c r="H4" s="12">
+        <v>2</v>
+      </c>
+      <c r="I4" s="12">
+        <v>9</v>
+      </c>
+      <c r="J4" s="12">
+        <v>13</v>
+      </c>
+      <c r="K4" s="12">
+        <v>22</v>
+      </c>
+      <c r="L4" s="12">
+        <v>28</v>
+      </c>
+      <c r="M4" s="12">
+        <v>2</v>
+      </c>
+      <c r="N4" s="12">
+        <v>36</v>
+      </c>
+      <c r="O4" s="12">
+        <v>45</v>
+      </c>
+      <c r="P4" s="12">
+        <v>49</v>
+      </c>
+      <c r="Q4" s="12">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>5</v>
       </c>
@@ -1988,42 +2056,44 @@
         <v>48</v>
       </c>
       <c r="C5" s="6">
-        <f>COUNTIF($E$2:$AH$61, A5)</f>
-        <v>2</v>
-      </c>
-      <c r="E5" s="2">
-        <v>11</v>
-      </c>
-      <c r="F5" s="2">
-        <v>5</v>
-      </c>
-      <c r="G5" s="2">
-        <v>11</v>
-      </c>
-      <c r="H5" s="2">
-        <v>15</v>
-      </c>
-      <c r="I5" s="2">
-        <v>24</v>
-      </c>
-      <c r="J5" s="2">
-        <v>30</v>
-      </c>
-      <c r="K5" s="2">
-        <v>5</v>
-      </c>
-      <c r="L5" s="2">
-        <v>38</v>
-      </c>
-      <c r="M5" s="2">
-        <v>42</v>
-      </c>
-      <c r="N5" s="2">
-        <v>51</v>
-      </c>
-      <c r="O5" s="2"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="12">
+        <v>10</v>
+      </c>
+      <c r="H5" s="12">
+        <v>3</v>
+      </c>
+      <c r="I5" s="12">
+        <v>10</v>
+      </c>
+      <c r="J5" s="12">
+        <v>14</v>
+      </c>
+      <c r="K5" s="12">
+        <v>23</v>
+      </c>
+      <c r="L5" s="12">
+        <v>29</v>
+      </c>
+      <c r="M5" s="12">
+        <v>3</v>
+      </c>
+      <c r="N5" s="12">
+        <v>37</v>
+      </c>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12">
+        <v>50</v>
+      </c>
+      <c r="Q5" s="12">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>6</v>
       </c>
@@ -2031,40 +2101,42 @@
         <v>49</v>
       </c>
       <c r="C6" s="6">
-        <f>COUNTIF($E$2:$AH$61, A6)</f>
-        <v>2</v>
-      </c>
-      <c r="E6" s="2">
-        <v>12</v>
-      </c>
-      <c r="F6" s="2">
-        <v>6</v>
-      </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2">
-        <v>16</v>
-      </c>
-      <c r="I6" s="2">
-        <v>26</v>
-      </c>
-      <c r="J6" s="2">
-        <v>31</v>
-      </c>
-      <c r="K6" s="2">
-        <v>6</v>
-      </c>
-      <c r="L6" s="2">
-        <v>39</v>
-      </c>
-      <c r="M6" s="2">
-        <v>44</v>
-      </c>
-      <c r="N6" s="2">
-        <v>52</v>
-      </c>
-      <c r="O6" s="2"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="12">
+        <v>11</v>
+      </c>
+      <c r="H6" s="12">
+        <v>5</v>
+      </c>
+      <c r="I6" s="12">
+        <v>11</v>
+      </c>
+      <c r="J6" s="12">
+        <v>15</v>
+      </c>
+      <c r="K6" s="12">
+        <v>24</v>
+      </c>
+      <c r="L6" s="12">
+        <v>30</v>
+      </c>
+      <c r="M6" s="12">
+        <v>5</v>
+      </c>
+      <c r="N6" s="12">
+        <v>38</v>
+      </c>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12">
+        <v>51</v>
+      </c>
+      <c r="Q6" s="12"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>7</v>
       </c>
@@ -2072,40 +2144,40 @@
         <v>50</v>
       </c>
       <c r="C7" s="6">
-        <f>COUNTIF($E$2:$AH$61, A7)</f>
-        <v>2</v>
-      </c>
-      <c r="E7" s="2">
-        <v>13</v>
-      </c>
-      <c r="F7" s="2">
-        <v>4</v>
-      </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2">
-        <v>17</v>
-      </c>
-      <c r="I7" s="2">
-        <v>25</v>
-      </c>
-      <c r="J7" s="2">
-        <v>32</v>
-      </c>
-      <c r="K7" s="2">
-        <v>4</v>
-      </c>
-      <c r="L7" s="2">
-        <v>40</v>
-      </c>
-      <c r="M7" s="2">
-        <v>46</v>
-      </c>
-      <c r="N7" s="2">
-        <v>53</v>
-      </c>
-      <c r="O7" s="2"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="12">
+        <v>12</v>
+      </c>
+      <c r="H7" s="12">
+        <v>6</v>
+      </c>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12">
+        <v>16</v>
+      </c>
+      <c r="K7" s="12">
+        <v>26</v>
+      </c>
+      <c r="L7" s="12">
+        <v>31</v>
+      </c>
+      <c r="M7" s="12">
+        <v>6</v>
+      </c>
+      <c r="N7" s="12">
+        <v>39</v>
+      </c>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12">
+        <v>52</v>
+      </c>
+      <c r="Q7" s="12"/>
+    </row>
+    <row r="8" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>8</v>
       </c>
@@ -2113,34 +2185,40 @@
         <v>51</v>
       </c>
       <c r="C8" s="6">
-        <f>COUNTIF($E$2:$AH$61, A8)</f>
-        <v>2</v>
-      </c>
-      <c r="E8" s="2">
-        <v>14</v>
-      </c>
-      <c r="F8" s="2">
-        <v>7</v>
-      </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2">
-        <v>18</v>
-      </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2">
-        <v>33</v>
-      </c>
-      <c r="K8" s="2">
-        <v>7</v>
-      </c>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2">
-        <v>48</v>
-      </c>
-      <c r="O8" s="2"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="12">
+        <v>13</v>
+      </c>
+      <c r="H8" s="12">
+        <v>4</v>
+      </c>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12">
+        <v>17</v>
+      </c>
+      <c r="K8" s="12">
+        <v>25</v>
+      </c>
+      <c r="L8" s="12">
+        <v>32</v>
+      </c>
+      <c r="M8" s="12">
+        <v>4</v>
+      </c>
+      <c r="N8" s="12">
+        <v>40</v>
+      </c>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12">
+        <v>53</v>
+      </c>
+      <c r="Q8" s="12"/>
+    </row>
+    <row r="9" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>9</v>
       </c>
@@ -2148,29 +2226,34 @@
         <v>52</v>
       </c>
       <c r="C9" s="6">
-        <f>COUNTIF($E$2:$AH$61, A9)</f>
-        <v>2</v>
-      </c>
-      <c r="E9" s="2">
-        <v>15</v>
-      </c>
-      <c r="F9" s="2">
-        <v>35</v>
-      </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2">
-        <v>19</v>
-      </c>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2">
-        <v>34</v>
-      </c>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="O9" s="2"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="12">
+        <v>14</v>
+      </c>
+      <c r="H9" s="12">
+        <v>7</v>
+      </c>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12">
+        <v>18</v>
+      </c>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12">
+        <v>33</v>
+      </c>
+      <c r="M9" s="12">
+        <v>7</v>
+      </c>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
+    </row>
+    <row r="10" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>10</v>
       </c>
@@ -2178,28 +2261,30 @@
         <v>53</v>
       </c>
       <c r="C10" s="6">
-        <f>COUNTIF($E$2:$AH$61, A10)</f>
-        <v>2</v>
-      </c>
-      <c r="E10" s="2">
-        <v>16</v>
-      </c>
-      <c r="F10" s="2">
-        <v>36</v>
-      </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2">
-        <v>20</v>
-      </c>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="12">
+        <v>15</v>
+      </c>
+      <c r="H10" s="12">
+        <v>35</v>
+      </c>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12">
+        <v>34</v>
+      </c>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="12"/>
+    </row>
+    <row r="11" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>11</v>
       </c>
@@ -2207,17 +2292,28 @@
         <v>54</v>
       </c>
       <c r="C11" s="6">
-        <f>COUNTIF($E$2:$AH$61, A11)</f>
-        <v>2</v>
-      </c>
-      <c r="E11" s="2">
-        <v>17</v>
-      </c>
-      <c r="F11" s="2">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="12">
+        <v>16</v>
+      </c>
+      <c r="H11" s="12">
+        <v>36</v>
+      </c>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+    </row>
+    <row r="12" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>12</v>
       </c>
@@ -2225,17 +2321,30 @@
         <v>34</v>
       </c>
       <c r="C12" s="6">
-        <f>COUNTIF($E$2:$AH$61, A12)</f>
-        <v>2</v>
-      </c>
-      <c r="E12" s="2">
-        <v>18</v>
-      </c>
-      <c r="F12" s="2">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="12">
+        <v>17</v>
+      </c>
+      <c r="H12" s="12">
+        <v>37</v>
+      </c>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+    </row>
+    <row r="13" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>13</v>
       </c>
@@ -2243,17 +2352,28 @@
         <v>33</v>
       </c>
       <c r="C13" s="6">
-        <f>COUNTIF($E$2:$AH$61, A13)</f>
-        <v>2</v>
-      </c>
-      <c r="E13" s="2">
-        <v>19</v>
-      </c>
-      <c r="F13" s="2">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="12">
+        <v>18</v>
+      </c>
+      <c r="H13" s="12">
+        <v>38</v>
+      </c>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="5"/>
+    </row>
+    <row r="14" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>14</v>
       </c>
@@ -2261,17 +2381,28 @@
         <v>32</v>
       </c>
       <c r="C14" s="6">
-        <f>COUNTIF($E$2:$AH$61, A14)</f>
-        <v>2</v>
-      </c>
-      <c r="E14" s="2">
-        <v>20</v>
-      </c>
-      <c r="F14" s="2">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="12">
+        <v>21</v>
+      </c>
+      <c r="H14" s="12">
+        <v>39</v>
+      </c>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+      <c r="P14" s="5"/>
+      <c r="Q14" s="5"/>
+    </row>
+    <row r="15" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>15</v>
       </c>
@@ -2279,17 +2410,28 @@
         <v>55</v>
       </c>
       <c r="C15" s="6">
-        <f>COUNTIF($E$2:$AH$61, A15)</f>
-        <v>2</v>
-      </c>
-      <c r="E15" s="2">
-        <v>21</v>
-      </c>
-      <c r="F15" s="2">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="12">
+        <v>22</v>
+      </c>
+      <c r="H15" s="12">
+        <v>40</v>
+      </c>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+    </row>
+    <row r="16" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>16</v>
       </c>
@@ -2297,17 +2439,28 @@
         <v>31</v>
       </c>
       <c r="C16" s="6">
-        <f>COUNTIF($E$2:$AH$61, A16)</f>
-        <v>2</v>
-      </c>
-      <c r="E16" s="2">
-        <v>22</v>
-      </c>
-      <c r="F16" s="2">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="12">
+        <v>23</v>
+      </c>
+      <c r="H16" s="12">
+        <v>43</v>
+      </c>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="5"/>
+    </row>
+    <row r="17" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>17</v>
       </c>
@@ -2315,17 +2468,28 @@
         <v>56</v>
       </c>
       <c r="C17" s="6">
-        <f>COUNTIF($E$2:$AH$61, A17)</f>
-        <v>2</v>
-      </c>
-      <c r="E17" s="2">
-        <v>23</v>
-      </c>
-      <c r="F17" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="12">
+        <v>24</v>
+      </c>
+      <c r="H17" s="12">
+        <v>45</v>
+      </c>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
+    </row>
+    <row r="18" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>18</v>
       </c>
@@ -2333,17 +2497,28 @@
         <v>30</v>
       </c>
       <c r="C18" s="6">
-        <f>COUNTIF($E$2:$AH$61, A18)</f>
-        <v>2</v>
-      </c>
-      <c r="E18" s="2">
-        <v>24</v>
-      </c>
-      <c r="F18" s="2">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="12">
+        <v>26</v>
+      </c>
+      <c r="H18" s="12">
+        <v>47</v>
+      </c>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+    </row>
+    <row r="19" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>19</v>
       </c>
@@ -2351,17 +2526,28 @@
         <v>29</v>
       </c>
       <c r="C19" s="6">
-        <f>COUNTIF($E$2:$AH$61, A19)</f>
-        <v>2</v>
-      </c>
-      <c r="E19" s="2">
-        <v>26</v>
-      </c>
-      <c r="F19" s="2">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="12">
+        <v>25</v>
+      </c>
+      <c r="H19" s="12">
+        <v>49</v>
+      </c>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+    </row>
+    <row r="20" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>20</v>
       </c>
@@ -2369,17 +2555,28 @@
         <v>28</v>
       </c>
       <c r="C20" s="6">
-        <f>COUNTIF($E$2:$AH$61, A20)</f>
-        <v>2</v>
-      </c>
-      <c r="E20" s="2">
-        <v>25</v>
-      </c>
-      <c r="F20" s="2">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="12">
+        <v>27</v>
+      </c>
+      <c r="H20" s="12">
+        <v>50</v>
+      </c>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+    </row>
+    <row r="21" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>21</v>
       </c>
@@ -2387,17 +2584,28 @@
         <v>27</v>
       </c>
       <c r="C21" s="6">
-        <f>COUNTIF($E$2:$AH$61, A21)</f>
-        <v>2</v>
-      </c>
-      <c r="E21" s="2">
-        <v>27</v>
-      </c>
-      <c r="F21" s="2">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="12">
+        <v>28</v>
+      </c>
+      <c r="H21" s="12">
+        <v>51</v>
+      </c>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+    </row>
+    <row r="22" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>22</v>
       </c>
@@ -2405,17 +2613,28 @@
         <v>26</v>
       </c>
       <c r="C22" s="6">
-        <f>COUNTIF($E$2:$AH$61, A22)</f>
-        <v>2</v>
-      </c>
-      <c r="E22" s="2">
-        <v>28</v>
-      </c>
-      <c r="F22" s="2">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="12">
+        <v>29</v>
+      </c>
+      <c r="H22" s="12">
+        <v>52</v>
+      </c>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+    </row>
+    <row r="23" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>23</v>
       </c>
@@ -2423,17 +2642,28 @@
         <v>23</v>
       </c>
       <c r="C23" s="6">
-        <f>COUNTIF($E$2:$AH$61, A23)</f>
-        <v>2</v>
-      </c>
-      <c r="E23" s="2">
-        <v>29</v>
-      </c>
-      <c r="F23" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="12">
+        <v>30</v>
+      </c>
+      <c r="H23" s="12">
+        <v>53</v>
+      </c>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
+    </row>
+    <row r="24" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>24</v>
       </c>
@@ -2441,17 +2671,28 @@
         <v>25</v>
       </c>
       <c r="C24" s="6">
-        <f>COUNTIF($E$2:$AH$61, A24)</f>
-        <v>2</v>
-      </c>
-      <c r="E24" s="2">
-        <v>30</v>
-      </c>
-      <c r="F24" s="2">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="12">
+        <v>31</v>
+      </c>
+      <c r="H24" s="12">
+        <v>54</v>
+      </c>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="5"/>
+    </row>
+    <row r="25" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>25</v>
       </c>
@@ -2459,17 +2700,28 @@
         <v>24</v>
       </c>
       <c r="C25" s="6">
-        <f>COUNTIF($E$2:$AH$61, A25)</f>
-        <v>2</v>
-      </c>
-      <c r="E25" s="2">
-        <v>31</v>
-      </c>
-      <c r="F25" s="2">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="12">
+        <v>32</v>
+      </c>
+      <c r="H25" s="12">
+        <v>55</v>
+      </c>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="5"/>
+    </row>
+    <row r="26" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>26</v>
       </c>
@@ -2477,17 +2729,28 @@
         <v>57</v>
       </c>
       <c r="C26" s="6">
-        <f>COUNTIF($E$2:$AH$61, A26)</f>
-        <v>2</v>
-      </c>
-      <c r="E26" s="2">
-        <v>32</v>
-      </c>
-      <c r="F26" s="2">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="12">
+        <v>33</v>
+      </c>
+      <c r="H26" s="12">
+        <v>56</v>
+      </c>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
+      <c r="P26" s="5"/>
+      <c r="Q26" s="5"/>
+    </row>
+    <row r="27" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>27</v>
       </c>
@@ -2495,17 +2758,25 @@
         <v>22</v>
       </c>
       <c r="C27" s="6">
-        <f>COUNTIF($E$2:$AH$61, A27)</f>
-        <v>2</v>
-      </c>
-      <c r="E27" s="2">
-        <v>33</v>
-      </c>
-      <c r="F27" s="2">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="12">
+        <v>34</v>
+      </c>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="5"/>
+    </row>
+    <row r="28" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>28</v>
       </c>
@@ -2513,17 +2784,24 @@
         <v>19</v>
       </c>
       <c r="C28" s="6">
-        <f>COUNTIF($E$2:$AH$61, A28)</f>
-        <v>2</v>
-      </c>
-      <c r="E28" s="2">
-        <v>34</v>
-      </c>
-      <c r="F28" s="2">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="5"/>
+    </row>
+    <row r="29" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>29</v>
       </c>
@@ -2531,14 +2809,24 @@
         <v>58</v>
       </c>
       <c r="C29" s="6">
-        <f>COUNTIF($E$2:$AH$61, A29)</f>
-        <v>2</v>
-      </c>
-      <c r="F29" s="2">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="5"/>
+    </row>
+    <row r="30" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>30</v>
       </c>
@@ -2546,14 +2834,24 @@
         <v>59</v>
       </c>
       <c r="C30" s="6">
-        <f>COUNTIF($E$2:$AH$61, A30)</f>
-        <v>2</v>
-      </c>
-      <c r="F30" s="2">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
+      <c r="P30" s="5"/>
+      <c r="Q30" s="5"/>
+    </row>
+    <row r="31" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>31</v>
       </c>
@@ -2561,11 +2859,24 @@
         <v>60</v>
       </c>
       <c r="C31" s="6">
-        <f>COUNTIF($E$2:$AH$61, A31)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
+      <c r="P31" s="5"/>
+      <c r="Q31" s="5"/>
+    </row>
+    <row r="32" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>32</v>
       </c>
@@ -2573,11 +2884,24 @@
         <v>21</v>
       </c>
       <c r="C32" s="6">
-        <f>COUNTIF($E$2:$AH$61, A32)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="5"/>
+      <c r="P32" s="5"/>
+      <c r="Q32" s="5"/>
+    </row>
+    <row r="33" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>33</v>
       </c>
@@ -2585,11 +2909,24 @@
         <v>20</v>
       </c>
       <c r="C33" s="6">
-        <f>COUNTIF($E$2:$AH$61, A33)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="5"/>
+      <c r="P33" s="5"/>
+      <c r="Q33" s="5"/>
+    </row>
+    <row r="34" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>34</v>
       </c>
@@ -2597,11 +2934,24 @@
         <v>61</v>
       </c>
       <c r="C34" s="6">
-        <f>COUNTIF($E$2:$AH$61, A34)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5"/>
+      <c r="O34" s="5"/>
+      <c r="P34" s="5"/>
+      <c r="Q34" s="5"/>
+    </row>
+    <row r="35" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>35</v>
       </c>
@@ -2609,11 +2959,24 @@
         <v>18</v>
       </c>
       <c r="C35" s="6">
-        <f>COUNTIF($E$2:$AH$61, A35)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+      <c r="N35" s="5"/>
+      <c r="O35" s="5"/>
+      <c r="P35" s="5"/>
+      <c r="Q35" s="5"/>
+    </row>
+    <row r="36" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>36</v>
       </c>
@@ -2621,11 +2984,24 @@
         <v>17</v>
       </c>
       <c r="C36" s="6">
-        <f>COUNTIF($E$2:$AH$61, A36)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="5"/>
+      <c r="O36" s="5"/>
+      <c r="P36" s="5"/>
+      <c r="Q36" s="5"/>
+    </row>
+    <row r="37" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>37</v>
       </c>
@@ -2633,11 +3009,24 @@
         <v>16</v>
       </c>
       <c r="C37" s="6">
-        <f>COUNTIF($E$2:$AH$61, A37)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="5"/>
+      <c r="M37" s="5"/>
+      <c r="N37" s="5"/>
+      <c r="O37" s="5"/>
+      <c r="P37" s="5"/>
+      <c r="Q37" s="5"/>
+    </row>
+    <row r="38" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>38</v>
       </c>
@@ -2645,11 +3034,24 @@
         <v>15</v>
       </c>
       <c r="C38" s="6">
-        <f>COUNTIF($E$2:$AH$61, A38)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5"/>
+      <c r="M38" s="5"/>
+      <c r="N38" s="5"/>
+      <c r="O38" s="5"/>
+      <c r="P38" s="5"/>
+      <c r="Q38" s="5"/>
+    </row>
+    <row r="39" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>39</v>
       </c>
@@ -2657,11 +3059,24 @@
         <v>14</v>
       </c>
       <c r="C39" s="6">
-        <f>COUNTIF($E$2:$AH$61, A39)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="5"/>
+      <c r="M39" s="5"/>
+      <c r="N39" s="5"/>
+      <c r="O39" s="5"/>
+      <c r="P39" s="5"/>
+      <c r="Q39" s="5"/>
+    </row>
+    <row r="40" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>40</v>
       </c>
@@ -2669,11 +3084,24 @@
         <v>12</v>
       </c>
       <c r="C40" s="6">
-        <f>COUNTIF($E$2:$AH$61, A40)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="5"/>
+      <c r="M40" s="5"/>
+      <c r="N40" s="5"/>
+      <c r="O40" s="5"/>
+      <c r="P40" s="5"/>
+      <c r="Q40" s="5"/>
+    </row>
+    <row r="41" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>41</v>
       </c>
@@ -2681,11 +3109,24 @@
         <v>13</v>
       </c>
       <c r="C41" s="6">
-        <f>COUNTIF($E$2:$AH$61, A41)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5"/>
+      <c r="M41" s="5"/>
+      <c r="N41" s="5"/>
+      <c r="O41" s="5"/>
+      <c r="P41" s="5"/>
+      <c r="Q41" s="5"/>
+    </row>
+    <row r="42" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>42</v>
       </c>
@@ -2693,11 +3134,24 @@
         <v>8</v>
       </c>
       <c r="C42" s="6">
-        <f>COUNTIF($E$2:$AH$61, A42)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="5"/>
+      <c r="L42" s="5"/>
+      <c r="M42" s="5"/>
+      <c r="N42" s="5"/>
+      <c r="O42" s="5"/>
+      <c r="P42" s="5"/>
+      <c r="Q42" s="5"/>
+    </row>
+    <row r="43" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>43</v>
       </c>
@@ -2705,11 +3159,24 @@
         <v>11</v>
       </c>
       <c r="C43" s="6">
-        <f>COUNTIF($E$2:$AH$61, A43)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5"/>
+      <c r="N43" s="5"/>
+      <c r="O43" s="5"/>
+      <c r="P43" s="5"/>
+      <c r="Q43" s="5"/>
+    </row>
+    <row r="44" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>44</v>
       </c>
@@ -2717,11 +3184,24 @@
         <v>10</v>
       </c>
       <c r="C44" s="6">
-        <f>COUNTIF($E$2:$AH$61, A44)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="5"/>
+      <c r="L44" s="5"/>
+      <c r="M44" s="5"/>
+      <c r="N44" s="5"/>
+      <c r="O44" s="5"/>
+      <c r="P44" s="5"/>
+      <c r="Q44" s="5"/>
+    </row>
+    <row r="45" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>45</v>
       </c>
@@ -2729,11 +3209,24 @@
         <v>62</v>
       </c>
       <c r="C45" s="6">
-        <f>COUNTIF($E$2:$AH$61, A45)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="5"/>
+      <c r="M45" s="5"/>
+      <c r="N45" s="5"/>
+      <c r="O45" s="5"/>
+      <c r="P45" s="5"/>
+      <c r="Q45" s="5"/>
+    </row>
+    <row r="46" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>46</v>
       </c>
@@ -2741,11 +3234,24 @@
         <v>9</v>
       </c>
       <c r="C46" s="6">
-        <f>COUNTIF($E$2:$AH$61, A46)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="5"/>
+      <c r="L46" s="5"/>
+      <c r="M46" s="5"/>
+      <c r="N46" s="5"/>
+      <c r="O46" s="5"/>
+      <c r="P46" s="5"/>
+      <c r="Q46" s="5"/>
+    </row>
+    <row r="47" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>47</v>
       </c>
@@ -2753,11 +3259,24 @@
         <v>63</v>
       </c>
       <c r="C47" s="6">
-        <f>COUNTIF($E$2:$AH$61, A47)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="5"/>
+      <c r="M47" s="5"/>
+      <c r="N47" s="5"/>
+      <c r="O47" s="5"/>
+      <c r="P47" s="5"/>
+      <c r="Q47" s="5"/>
+    </row>
+    <row r="48" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>48</v>
       </c>
@@ -2765,11 +3284,24 @@
         <v>7</v>
       </c>
       <c r="C48" s="6">
-        <f>COUNTIF($E$2:$AH$61, A48)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="5"/>
+      <c r="J48" s="5"/>
+      <c r="K48" s="5"/>
+      <c r="L48" s="5"/>
+      <c r="M48" s="5"/>
+      <c r="N48" s="5"/>
+      <c r="O48" s="5"/>
+      <c r="P48" s="5"/>
+      <c r="Q48" s="5"/>
+    </row>
+    <row r="49" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>49</v>
       </c>
@@ -2777,11 +3309,24 @@
         <v>4</v>
       </c>
       <c r="C49" s="6">
-        <f>COUNTIF($E$2:$AH$61, A49)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="5"/>
+      <c r="J49" s="5"/>
+      <c r="K49" s="5"/>
+      <c r="L49" s="5"/>
+      <c r="M49" s="5"/>
+      <c r="N49" s="5"/>
+      <c r="O49" s="5"/>
+      <c r="P49" s="5"/>
+      <c r="Q49" s="5"/>
+    </row>
+    <row r="50" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>50</v>
       </c>
@@ -2789,11 +3334,24 @@
         <v>5</v>
       </c>
       <c r="C50" s="6">
-        <f>COUNTIF($E$2:$AH$61, A50)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="5"/>
+      <c r="J50" s="5"/>
+      <c r="K50" s="5"/>
+      <c r="L50" s="5"/>
+      <c r="M50" s="5"/>
+      <c r="N50" s="5"/>
+      <c r="O50" s="5"/>
+      <c r="P50" s="5"/>
+      <c r="Q50" s="5"/>
+    </row>
+    <row r="51" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>51</v>
       </c>
@@ -2801,11 +3359,24 @@
         <v>64</v>
       </c>
       <c r="C51" s="6">
-        <f>COUNTIF($E$2:$AH$61, A51)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5"/>
+      <c r="I51" s="5"/>
+      <c r="J51" s="5"/>
+      <c r="K51" s="5"/>
+      <c r="L51" s="5"/>
+      <c r="M51" s="5"/>
+      <c r="N51" s="5"/>
+      <c r="O51" s="5"/>
+      <c r="P51" s="5"/>
+      <c r="Q51" s="5"/>
+    </row>
+    <row r="52" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>52</v>
       </c>
@@ -2813,11 +3384,24 @@
         <v>3</v>
       </c>
       <c r="C52" s="6">
-        <f>COUNTIF($E$2:$AH$61, A52)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="5"/>
+      <c r="I52" s="5"/>
+      <c r="J52" s="5"/>
+      <c r="K52" s="5"/>
+      <c r="L52" s="5"/>
+      <c r="M52" s="5"/>
+      <c r="N52" s="5"/>
+      <c r="O52" s="5"/>
+      <c r="P52" s="5"/>
+      <c r="Q52" s="5"/>
+    </row>
+    <row r="53" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>53</v>
       </c>
@@ -2825,11 +3409,24 @@
         <v>6</v>
       </c>
       <c r="C53" s="6">
-        <f>COUNTIF($E$2:$AH$61, A53)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="5"/>
+      <c r="J53" s="5"/>
+      <c r="K53" s="5"/>
+      <c r="L53" s="5"/>
+      <c r="M53" s="5"/>
+      <c r="N53" s="5"/>
+      <c r="O53" s="5"/>
+      <c r="P53" s="5"/>
+      <c r="Q53" s="5"/>
+    </row>
+    <row r="54" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>54</v>
       </c>
@@ -2837,11 +3434,24 @@
         <v>1</v>
       </c>
       <c r="C54" s="6">
-        <f>COUNTIF($E$2:$AH$61, A54)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="5"/>
+      <c r="I54" s="5"/>
+      <c r="J54" s="5"/>
+      <c r="K54" s="5"/>
+      <c r="L54" s="5"/>
+      <c r="M54" s="5"/>
+      <c r="N54" s="5"/>
+      <c r="O54" s="5"/>
+      <c r="P54" s="5"/>
+      <c r="Q54" s="5"/>
+    </row>
+    <row r="55" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>55</v>
       </c>
@@ -2849,11 +3459,24 @@
         <v>0</v>
       </c>
       <c r="C55" s="6">
-        <f>COUNTIF($E$2:$AH$61, A55)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5"/>
+      <c r="H55" s="5"/>
+      <c r="I55" s="5"/>
+      <c r="J55" s="5"/>
+      <c r="K55" s="5"/>
+      <c r="L55" s="5"/>
+      <c r="M55" s="5"/>
+      <c r="N55" s="5"/>
+      <c r="O55" s="5"/>
+      <c r="P55" s="5"/>
+      <c r="Q55" s="5"/>
+    </row>
+    <row r="56" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>56</v>
       </c>
@@ -2861,49 +3484,114 @@
         <v>2</v>
       </c>
       <c r="C56" s="6">
-        <f>COUNTIF($E$2:$AH$61, A56)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5"/>
+      <c r="H56" s="5"/>
+      <c r="I56" s="5"/>
+      <c r="J56" s="5"/>
+      <c r="K56" s="5"/>
+      <c r="L56" s="5"/>
+      <c r="M56" s="5"/>
+      <c r="N56" s="5"/>
+      <c r="O56" s="5"/>
+      <c r="P56" s="5"/>
+      <c r="Q56" s="5"/>
+    </row>
+    <row r="57" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>57</v>
       </c>
       <c r="B57" s="5"/>
       <c r="C57" s="6">
-        <f>COUNTIF($E$2:$AH$61, A57)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="5"/>
+      <c r="I57" s="5"/>
+      <c r="J57" s="5"/>
+      <c r="K57" s="5"/>
+      <c r="L57" s="5"/>
+      <c r="M57" s="5"/>
+      <c r="N57" s="5"/>
+      <c r="O57" s="5"/>
+      <c r="P57" s="5"/>
+      <c r="Q57" s="5"/>
+    </row>
+    <row r="58" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>58</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="6">
-        <f>COUNTIF($E$2:$AH$61, A58)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="5"/>
+      <c r="I58" s="5"/>
+      <c r="J58" s="5"/>
+      <c r="K58" s="5"/>
+      <c r="L58" s="5"/>
+      <c r="M58" s="5"/>
+      <c r="N58" s="5"/>
+      <c r="O58" s="5"/>
+      <c r="P58" s="5"/>
+      <c r="Q58" s="5"/>
+    </row>
+    <row r="59" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>59</v>
       </c>
       <c r="B59" s="5"/>
       <c r="C59" s="6">
-        <f>COUNTIF($E$2:$AH$61, A59)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
+      <c r="H59" s="5"/>
+      <c r="I59" s="5"/>
+      <c r="J59" s="5"/>
+      <c r="K59" s="5"/>
+      <c r="L59" s="5"/>
+      <c r="M59" s="5"/>
+      <c r="N59" s="5"/>
+      <c r="O59" s="5"/>
+      <c r="P59" s="5"/>
+      <c r="Q59" s="5"/>
+    </row>
+    <row r="60" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>60</v>
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="6">
-        <f>COUNTIF($E$2:$AH$61, A60)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+      <c r="H60" s="5"/>
+      <c r="I60" s="5"/>
+      <c r="J60" s="5"/>
+      <c r="K60" s="5"/>
+      <c r="L60" s="5"/>
+      <c r="M60" s="5"/>
+      <c r="N60" s="5"/>
+      <c r="O60" s="5"/>
+      <c r="P60" s="5"/>
+      <c r="Q60" s="5"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:C60">

</xml_diff>

<commit_message>
Various lag specifications added, new optimization of A matrix
</commit_message>
<xml_diff>
--- a/Block_WBC.xlsx
+++ b/Block_WBC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sigve Borgmo\OneDrive - NTNU\Indok\Master\dynamic-factor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E35C3127-1947-4155-9B78-48530E6DFBFE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D736B8B7-DC08-4B6F-B202-B5CB19B8C3C1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1826,7 +1826,7 @@
   <dimension ref="A1:Q60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="H2" sqref="H2:Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1914,43 +1914,43 @@
         <v>68</v>
       </c>
       <c r="F2" s="10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G2" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H2" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I2" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J2" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K2" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L2" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M2" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N2" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O2" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P2" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q2" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>3</v>
       </c>
@@ -2001,7 +2001,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>4</v>
       </c>
@@ -2048,7 +2048,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>5</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>6</v>
       </c>

</xml_diff>